<commit_message>
Added more efficient algorithm
</commit_message>
<xml_diff>
--- a/Projekt2_Liczby_Pierwsze/Projekt2-dane.xlsx
+++ b/Projekt2_Liczby_Pierwsze/Projekt2-dane.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>Number</t>
   </si>
@@ -42,6 +42,12 @@
   </si>
   <si>
     <t>PrimeNumbersPositive - Instr</t>
+  </si>
+  <si>
+    <t>PrimeNumbersOptimal - Time</t>
+  </si>
+  <si>
+    <t>PrimeNumbersOptimal - Instr</t>
   </si>
 </sst>
 </file>
@@ -396,7 +402,7 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -404,6 +410,7 @@
     <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="28.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="39" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="39.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
     <col min="10" max="10" width="18.7109375" customWidth="1"/>
@@ -422,7 +429,9 @@
       <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2"/>
+      <c r="D1" s="7" t="s">
+        <v>6</v>
+      </c>
       <c r="E1" s="5"/>
       <c r="F1" s="5"/>
     </row>
@@ -436,7 +445,9 @@
       <c r="C2" s="6">
         <v>0</v>
       </c>
-      <c r="D2" s="2"/>
+      <c r="D2" s="1">
+        <v>0</v>
+      </c>
       <c r="E2" s="2"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -449,6 +460,9 @@
       <c r="C3" s="6">
         <v>0</v>
       </c>
+      <c r="D3" s="1">
+        <v>0</v>
+      </c>
       <c r="E3" s="1"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -461,6 +475,9 @@
       <c r="C4" s="6">
         <v>0</v>
       </c>
+      <c r="D4" s="1">
+        <v>0</v>
+      </c>
       <c r="E4" s="1"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -473,6 +490,9 @@
       <c r="C5" s="6">
         <v>0</v>
       </c>
+      <c r="D5" s="1">
+        <v>0</v>
+      </c>
       <c r="E5" s="1"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -485,6 +505,9 @@
       <c r="C6" s="6">
         <v>0</v>
       </c>
+      <c r="D6" s="1">
+        <v>0</v>
+      </c>
       <c r="E6" s="1"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -497,6 +520,9 @@
       <c r="C7" s="6">
         <v>2</v>
       </c>
+      <c r="D7" s="1">
+        <v>1</v>
+      </c>
       <c r="E7" s="1"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -507,6 +533,9 @@
       <c r="C8" s="6">
         <v>6</v>
       </c>
+      <c r="D8" s="1">
+        <v>5</v>
+      </c>
       <c r="E8" s="1"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -516,6 +545,9 @@
       <c r="B9" s="4"/>
       <c r="C9" s="6">
         <v>19</v>
+      </c>
+      <c r="D9" s="1">
+        <v>15</v>
       </c>
       <c r="E9" s="1"/>
     </row>
@@ -546,7 +578,9 @@
       <c r="C13" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="2"/>
+      <c r="D13" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -559,7 +593,9 @@
       <c r="C14" s="6">
         <v>159</v>
       </c>
-      <c r="D14" s="2"/>
+      <c r="D14" s="6">
+        <v>108</v>
+      </c>
       <c r="E14" s="2"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -572,6 +608,9 @@
       <c r="C15" s="6">
         <v>502</v>
       </c>
+      <c r="D15" s="6">
+        <v>337</v>
+      </c>
       <c r="E15" s="1"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -584,6 +623,9 @@
       <c r="C16" s="6">
         <v>1588</v>
       </c>
+      <c r="D16" s="6">
+        <v>1061</v>
+      </c>
       <c r="E16" s="1"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -596,6 +638,9 @@
       <c r="C17" s="6">
         <v>5023</v>
       </c>
+      <c r="D17" s="6">
+        <v>3351</v>
+      </c>
       <c r="E17" s="1"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -608,6 +653,9 @@
       <c r="C18" s="6">
         <v>15883</v>
       </c>
+      <c r="D18" s="6">
+        <v>10591</v>
+      </c>
       <c r="E18" s="1"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -620,6 +668,9 @@
       <c r="C19" s="6">
         <v>50228</v>
       </c>
+      <c r="D19" s="6">
+        <v>33487</v>
+      </c>
       <c r="E19" s="1"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -632,6 +683,9 @@
       <c r="C20" s="6">
         <v>158835</v>
       </c>
+      <c r="D20" s="6">
+        <v>105892</v>
+      </c>
       <c r="E20" s="1"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -643,6 +697,9 @@
       </c>
       <c r="C21" s="6">
         <v>502280</v>
+      </c>
+      <c r="D21" s="6">
+        <v>334855</v>
       </c>
       <c r="E21" s="1"/>
     </row>

</xml_diff>